<commit_message>
Improved quiz response. Now you can get all the possible answers. Also added potato response
</commit_message>
<xml_diff>
--- a/quiz.xlsx
+++ b/quiz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thien\Desktop\coding_projects\Mathbot_real\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A19ED21-2D58-4210-A9E3-41F467D5153C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4D84D8-D051-4279-A33B-EE4FCD55F6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="528" yWindow="1644" windowWidth="17232" windowHeight="12012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="444" yWindow="0" windowWidth="17232" windowHeight="12012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -196,7 +196,62 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -207,6 +262,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{970288C7-B3C6-4FC2-9913-A682462EF451}" name="Table1" displayName="Table1" ref="A1:B20" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:B20" xr:uid="{970288C7-B3C6-4FC2-9913-A682462EF451}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
+    <sortCondition ref="A1:A20"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{9EA25EF3-40B8-4642-ABA8-516FA680C781}" name="Question" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{7B97CBE1-6670-4DB8-B44B-24FA1025B13F}" name="Answer" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,12 +544,13 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="62" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -493,157 +563,160 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
+      <c r="A8" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>30</v>
+      <c r="A17" t="s">
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>38</v>
+      <c r="A20" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added possibility to create bingo plates
</commit_message>
<xml_diff>
--- a/quiz.xlsx
+++ b/quiz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thien\Desktop\coding_projects\Mathbot_real\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89010334-B8C3-4327-868F-24A85B1989D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638ABD64-91A1-4E29-8550-65E62809B023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="228" windowWidth="17220" windowHeight="12012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10872" yWindow="1020" windowWidth="17232" windowHeight="12012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>You can smell me, and see me, but please dont touch me. What am I?</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Fluesopp</t>
   </si>
   <si>
-    <t>I am representing friendship, what am I?</t>
-  </si>
-  <si>
     <t>Vennestatue</t>
   </si>
   <si>
@@ -151,6 +148,21 @@
   </si>
   <si>
     <t>Rød ballong</t>
+  </si>
+  <si>
+    <t>In the end, there is always gold. What am I?</t>
+  </si>
+  <si>
+    <t>Regnbue</t>
+  </si>
+  <si>
+    <t>A building with a lot of story, what am I?</t>
+  </si>
+  <si>
+    <t>Pyramide</t>
+  </si>
+  <si>
+    <t>Im representing friendship, what am I?</t>
   </si>
 </sst>
 </file>
@@ -271,10 +283,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{970288C7-B3C6-4FC2-9913-A682462EF451}" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A1:B21" xr:uid="{970288C7-B3C6-4FC2-9913-A682462EF451}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B21">
-    <sortCondition ref="A1:A21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{970288C7-B3C6-4FC2-9913-A682462EF451}" name="Table1" displayName="Table1" ref="A1:B23" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="A1:B23" xr:uid="{970288C7-B3C6-4FC2-9913-A682462EF451}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B23">
+    <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{9EA25EF3-40B8-4642-ABA8-516FA680C781}" name="Question" dataDxfId="1"/>
@@ -547,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,176 +573,197 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>38</v>
+      <c r="A18" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
+      <c r="A20" t="s">
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>